<commit_message>
Add loop with data_browser, browser_rating
</commit_message>
<xml_diff>
--- a/xlsxtest.xlsx
+++ b/xlsxtest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pythonprojects\lessonpandashome\lessonpandas\lessonpandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD67597-09ED-4BE0-94FC-9FD4DF3EC24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8771A1-256A-4175-AC9C-24DB7D2C6738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11835" xr2:uid="{08E7A9E1-773C-4F6B-A08C-E2C42A7BE10E}"/>
+    <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11835" xr2:uid="{08E7A9E1-773C-4F6B-A08C-E2C42A7BE10E}"/>
   </bookViews>
   <sheets>
     <sheet name="log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>IP-адрес</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>Самый невостребованный товар среди женщин</t>
+  </si>
+  <si>
+    <t>188.170.85.xxx</t>
+  </si>
+  <si>
+    <t>Mobile Safari 13</t>
+  </si>
+  <si>
+    <t>00:06:06</t>
+  </si>
+  <si>
+    <t>Браслет Xiaomi Mi Band 4 Deep space blue,ArtSpace Набор обложек для дневников и тетрадей 210x350 мм,Berlingo Мешок для обуви Dream Unicorn (MS09230) фиолетовый</t>
   </si>
 </sst>
 </file>
@@ -372,11 +384,8 @@
     </xf>
     <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -417,6 +426,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -735,176 +750,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF3B423-B82C-4315-9417-2CF5F43B39FA}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="18" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>67</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>43914</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>66</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="5">
         <v>44021</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>59</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>43974</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>62</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>43864</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>66</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>43869</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="5">
+        <v>43921</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -923,590 +969,590 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="27" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="1:13" ht="27" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" spans="1:13" ht="27" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="B3" s="18" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="18"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
     </row>
     <row r="9" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
     </row>
     <row r="10" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
     </row>
     <row r="11" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="16"/>
-      <c r="L12" s="16"/>
-      <c r="M12" s="16"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
     </row>
     <row r="13" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" ht="27" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:13" ht="27" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" ht="27" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="18" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="18"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="G18" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="K18" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L18" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M18" s="11" t="s">
+      <c r="M18" s="10" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
     </row>
     <row r="20" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
     </row>
     <row r="21" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
     </row>
     <row r="22" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
     </row>
     <row r="23" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
     </row>
     <row r="24" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="15"/>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
     </row>
     <row r="25" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
     </row>
     <row r="26" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
-      <c r="K26" s="16"/>
-      <c r="L26" s="16"/>
-      <c r="M26" s="16"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
     </row>
     <row r="27" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" ht="27" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
     </row>
     <row r="29" spans="1:13" ht="27" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
-      <c r="M29" s="8"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
     </row>
     <row r="30" spans="1:13" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="17" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="8"/>
-      <c r="M30" s="8"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
     </row>
     <row r="31" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-      <c r="M31" s="8"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
     </row>
     <row r="32" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="A32" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
-      <c r="M32" s="8"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
     </row>
     <row r="33" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
-      <c r="M33" s="8"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
     </row>
     <row r="34" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
-      <c r="M34" s="8"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Third copy with dicts browsers and goods for other pc
</commit_message>
<xml_diff>
--- a/xlsxtest.xlsx
+++ b/xlsxtest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pythonprojects\lessonpandashome\lessonpandas\lessonpandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8771A1-256A-4175-AC9C-24DB7D2C6738}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760059DB-90E2-4751-8C9B-6F62B6870328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="2595" windowWidth="21600" windowHeight="11835" xr2:uid="{08E7A9E1-773C-4F6B-A08C-E2C42A7BE10E}"/>
+    <workbookView xWindow="3165" yWindow="2490" windowWidth="21600" windowHeight="11835" xr2:uid="{08E7A9E1-773C-4F6B-A08C-E2C42A7BE10E}"/>
   </bookViews>
   <sheets>
     <sheet name="log" sheetId="1" r:id="rId1"/>
@@ -218,7 +218,7 @@
     <t>00:06:06</t>
   </si>
   <si>
-    <t>Браслет Xiaomi Mi Band 4 Deep space blue,ArtSpace Набор обложек для дневников и тетрадей 210x350 мм,Berlingo Мешок для обуви Dream Unicorn (MS09230) фиолетовый</t>
+    <t>Сменный ремешок для Xiaomi Mi Band 4 и Mi Band 3 Черный,Браслет Xiaomi Mi Band 4 Deep space blue,ArtSpace Набор обложек для дневников и тетрадей 210x350 мм,Berlingo Мешок для обуви Dream Unicorn (MS09230) фиолетовый</t>
   </si>
 </sst>
 </file>
@@ -424,14 +424,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -753,7 +753,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,29 +766,29 @@
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:8" s="18" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1002,20 +1002,20 @@
     </row>
     <row r="3" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A3" s="8"/>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1244,20 +1244,20 @@
     </row>
     <row r="17" spans="1:13" ht="27" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">

</xml_diff>

<commit_message>
Add file utils with function - all_browsers, visits_of_browsers, all_goods, buying, mens_choice, women_choice
</commit_message>
<xml_diff>
--- a/xlsxtest.xlsx
+++ b/xlsxtest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pythonprojects\lessonpandashome\lessonpandas\lessonpandas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760059DB-90E2-4751-8C9B-6F62B6870328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E85197B-BA39-4CA6-B7A2-9370B882CEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3165" yWindow="2490" windowWidth="21600" windowHeight="11835" xr2:uid="{08E7A9E1-773C-4F6B-A08C-E2C42A7BE10E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{08E7A9E1-773C-4F6B-A08C-E2C42A7BE10E}"/>
   </bookViews>
   <sheets>
     <sheet name="log" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
   <si>
     <t>IP-адрес</t>
   </si>
@@ -219,6 +219,9 @@
   </si>
   <si>
     <t>Сменный ремешок для Xiaomi Mi Band 4 и Mi Band 3 Черный,Браслет Xiaomi Mi Band 4 Deep space blue,ArtSpace Набор обложек для дневников и тетрадей 210x350 мм,Berlingo Мешок для обуви Dream Unicorn (MS09230) фиолетовый</t>
+  </si>
+  <si>
+    <t>ж</t>
   </si>
 </sst>
 </file>
@@ -753,7 +756,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +930,7 @@
         <v>57</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="C7" s="2">
         <v>21</v>

</xml_diff>